<commit_message>
Fixed the command for how we change the player weapons over
</commit_message>
<xml_diff>
--- a/resources/data-imports/Weapons/specialty_weapons.xlsx
+++ b/resources/data-imports/Weapons/specialty_weapons.xlsx
@@ -1175,8 +1175,8 @@
   </sheetPr>
   <dimension ref="A1:BX1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H99" activeCellId="0" sqref="H99"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A81" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3277,9 +3277,6 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C16" s="1" t="s">
         <v>113</v>
       </c>
@@ -3408,9 +3405,6 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
-        <v>680</v>
-      </c>
       <c r="C17" s="1" t="s">
         <v>116</v>
       </c>
@@ -3539,9 +3533,6 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
-        <v>681</v>
-      </c>
       <c r="C18" s="1" t="s">
         <v>118</v>
       </c>
@@ -3670,9 +3661,6 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C19" s="1" t="s">
         <v>120</v>
       </c>
@@ -3801,9 +3789,6 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C20" s="1" t="s">
         <v>122</v>
       </c>
@@ -3932,9 +3917,6 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C21" s="1" t="s">
         <v>124</v>
       </c>
@@ -4063,9 +4045,6 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C22" s="1" t="s">
         <v>126</v>
       </c>
@@ -4194,9 +4173,6 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C23" s="1" t="s">
         <v>128</v>
       </c>
@@ -4325,9 +4301,6 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
-        <v>680</v>
-      </c>
       <c r="C24" s="1" t="s">
         <v>131</v>
       </c>
@@ -4456,9 +4429,6 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
-        <v>681</v>
-      </c>
       <c r="C25" s="1" t="s">
         <v>133</v>
       </c>
@@ -4587,9 +4557,6 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C26" s="1" t="s">
         <v>135</v>
       </c>
@@ -4718,9 +4685,6 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C27" s="1" t="s">
         <v>137</v>
       </c>
@@ -4849,9 +4813,6 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C28" s="1" t="s">
         <v>139</v>
       </c>
@@ -4980,9 +4941,6 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C29" s="1" t="s">
         <v>141</v>
       </c>
@@ -5111,9 +5069,6 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C30" s="1" t="s">
         <v>143</v>
       </c>
@@ -5242,9 +5197,6 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
-        <v>680</v>
-      </c>
       <c r="C31" s="1" t="s">
         <v>146</v>
       </c>
@@ -5373,9 +5325,6 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
-        <v>681</v>
-      </c>
       <c r="C32" s="1" t="s">
         <v>148</v>
       </c>
@@ -5504,9 +5453,6 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C33" s="1" t="s">
         <v>150</v>
       </c>
@@ -5635,9 +5581,6 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C34" s="1" t="s">
         <v>152</v>
       </c>
@@ -5766,9 +5709,6 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C35" s="1" t="s">
         <v>154</v>
       </c>
@@ -5897,9 +5837,6 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C36" s="1" t="s">
         <v>156</v>
       </c>
@@ -6028,9 +5965,6 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C37" s="1" t="s">
         <v>158</v>
       </c>
@@ -6159,9 +6093,6 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
-        <v>680</v>
-      </c>
       <c r="C38" s="1" t="s">
         <v>161</v>
       </c>
@@ -6290,9 +6221,6 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
-        <v>681</v>
-      </c>
       <c r="C39" s="1" t="s">
         <v>163</v>
       </c>
@@ -6421,9 +6349,6 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C40" s="1" t="s">
         <v>165</v>
       </c>
@@ -6552,9 +6477,6 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C41" s="1" t="s">
         <v>167</v>
       </c>
@@ -6683,9 +6605,6 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C42" s="1" t="s">
         <v>169</v>
       </c>
@@ -6814,9 +6733,6 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="n">
-        <v>679</v>
-      </c>
       <c r="C43" s="1" t="s">
         <v>171</v>
       </c>
@@ -6945,9 +6861,6 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
-        <v>687</v>
-      </c>
       <c r="C44" s="1" t="s">
         <v>173</v>
       </c>
@@ -7064,9 +6977,6 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="n">
-        <v>688</v>
-      </c>
       <c r="C45" s="1" t="s">
         <v>176</v>
       </c>
@@ -7183,9 +7093,6 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="n">
-        <v>689</v>
-      </c>
       <c r="C46" s="1" t="s">
         <v>178</v>
       </c>
@@ -7302,9 +7209,6 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
-        <v>687</v>
-      </c>
       <c r="C47" s="1" t="s">
         <v>180</v>
       </c>
@@ -7421,9 +7325,6 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
-        <v>687</v>
-      </c>
       <c r="C48" s="1" t="s">
         <v>182</v>
       </c>
@@ -7540,9 +7441,6 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
-        <v>687</v>
-      </c>
       <c r="C49" s="1" t="s">
         <v>184</v>
       </c>
@@ -7659,9 +7557,6 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="n">
-        <v>687</v>
-      </c>
       <c r="C50" s="1" t="s">
         <v>186</v>
       </c>
@@ -7778,9 +7673,6 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="n">
-        <v>687</v>
-      </c>
       <c r="C51" s="1" t="s">
         <v>188</v>
       </c>
@@ -7900,9 +7792,6 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="n">
-        <v>685</v>
-      </c>
       <c r="C52" s="1" t="s">
         <v>191</v>
       </c>
@@ -8022,9 +7911,6 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="n">
-        <v>686</v>
-      </c>
       <c r="C53" s="1" t="s">
         <v>193</v>
       </c>
@@ -8144,9 +8030,6 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="n">
-        <v>686</v>
-      </c>
       <c r="C54" s="1" t="s">
         <v>195</v>
       </c>
@@ -8266,9 +8149,6 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="1" t="n">
-        <v>686</v>
-      </c>
       <c r="C55" s="1" t="s">
         <v>197</v>
       </c>
@@ -8388,9 +8268,6 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="n">
-        <v>686</v>
-      </c>
       <c r="C56" s="1" t="s">
         <v>199</v>
       </c>
@@ -8510,9 +8387,6 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="n">
-        <v>686</v>
-      </c>
       <c r="C57" s="1" t="s">
         <v>201</v>
       </c>
@@ -10379,9 +10253,6 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="n">
-        <v>694</v>
-      </c>
       <c r="C72" s="1" t="s">
         <v>226</v>
       </c>
@@ -10498,9 +10369,6 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="n">
-        <v>695</v>
-      </c>
       <c r="C73" s="1" t="s">
         <v>229</v>
       </c>
@@ -10617,9 +10485,6 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="n">
-        <v>696</v>
-      </c>
       <c r="C74" s="1" t="s">
         <v>231</v>
       </c>
@@ -10736,9 +10601,6 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="n">
-        <v>694</v>
-      </c>
       <c r="C75" s="1" t="s">
         <v>233</v>
       </c>
@@ -10855,9 +10717,6 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="n">
-        <v>694</v>
-      </c>
       <c r="C76" s="1" t="s">
         <v>235</v>
       </c>
@@ -10974,9 +10833,6 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="n">
-        <v>694</v>
-      </c>
       <c r="C77" s="1" t="s">
         <v>237</v>
       </c>
@@ -11093,9 +10949,6 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="n">
-        <v>694</v>
-      </c>
       <c r="C78" s="1" t="s">
         <v>239</v>
       </c>
@@ -11212,9 +11065,6 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="n">
-        <v>691</v>
-      </c>
       <c r="C79" s="1" t="s">
         <v>241</v>
       </c>
@@ -11331,9 +11181,6 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="n">
-        <v>692</v>
-      </c>
       <c r="C80" s="1" t="s">
         <v>244</v>
       </c>
@@ -11450,9 +11297,6 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="n">
-        <v>693</v>
-      </c>
       <c r="C81" s="1" t="s">
         <v>246</v>
       </c>
@@ -11569,9 +11413,6 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="n">
-        <v>691</v>
-      </c>
       <c r="C82" s="1" t="s">
         <v>248</v>
       </c>
@@ -11688,9 +11529,6 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="n">
-        <v>691</v>
-      </c>
       <c r="C83" s="1" t="s">
         <v>250</v>
       </c>
@@ -11807,9 +11645,6 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="n">
-        <v>691</v>
-      </c>
       <c r="C84" s="1" t="s">
         <v>252</v>
       </c>
@@ -11926,9 +11761,6 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="n">
-        <v>691</v>
-      </c>
       <c r="C85" s="1" t="s">
         <v>254</v>
       </c>
@@ -12045,9 +11877,6 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="n">
-        <v>682</v>
-      </c>
       <c r="C86" s="1" t="s">
         <v>256</v>
       </c>
@@ -12164,9 +11993,6 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="n">
-        <v>683</v>
-      </c>
       <c r="C87" s="1" t="s">
         <v>259</v>
       </c>
@@ -12283,9 +12109,6 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="n">
-        <v>684</v>
-      </c>
       <c r="C88" s="1" t="s">
         <v>261</v>
       </c>
@@ -12402,9 +12225,6 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="n">
-        <v>682</v>
-      </c>
       <c r="C89" s="1" t="s">
         <v>263</v>
       </c>
@@ -12521,9 +12341,6 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="n">
-        <v>682</v>
-      </c>
       <c r="C90" s="1" t="s">
         <v>265</v>
       </c>
@@ -12640,9 +12457,6 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="n">
-        <v>682</v>
-      </c>
       <c r="C91" s="1" t="s">
         <v>267</v>
       </c>
@@ -12759,9 +12573,6 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="n">
-        <v>682</v>
-      </c>
       <c r="C92" s="1" t="s">
         <v>269</v>
       </c>

</xml_diff>